<commit_message>
data-model: Update with agreed data model
</commit_message>
<xml_diff>
--- a/indigo/spreadsheetform_guides/organisation.xlsx
+++ b/indigo/spreadsheetform_guides/organisation.xlsx
@@ -20,39 +20,42 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+  <si>
+    <t xml:space="preserve">Org-Ids</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Company</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPREADSHEETFORM:SINGLE:org-ids/company/value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Charity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPREADSHEETFORM:SINGLE:org-ids/charity/value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Other</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPREADSHEETFORM:SINGLE:org-ids/other/value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Contact</t>
+  </si>
   <si>
     <t xml:space="preserve">Name</t>
   </si>
   <si>
-    <t xml:space="preserve">SPREADSHEETFORM:SINGLE:name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SPREADSHEETFORM:SINGLE:type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Select</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Type1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Type2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Contact</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SPREADSHEETFORM:SINGLE:contact/name</t>
+    <t xml:space="preserve">SPREADSHEETFORM:SINGLE:contact/name/value</t>
   </si>
   <si>
     <t xml:space="preserve">Email</t>
   </si>
   <si>
-    <t xml:space="preserve">SPREADSHEETFORM:SINGLE:contact/email</t>
+    <t xml:space="preserve">SPREADSHEETFORM:SINGLE:contact/email/value</t>
   </si>
   <si>
     <t xml:space="preserve">Details</t>
@@ -61,7 +64,25 @@
     <t xml:space="preserve">Website</t>
   </si>
   <si>
-    <t xml:space="preserve">SPREADSHEETFORM:SINGLE:website</t>
+    <t xml:space="preserve">SPREADSHEETFORM:SINGLE:website/value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPREADSHEETFORM:SINGLE:address/value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Postcode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPREADSHEETFORM:SINGLE:postcode/value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Country</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPREADSHEETFORM:SINGLE:country/value</t>
   </si>
 </sst>
 </file>
@@ -270,10 +291,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:C35"/>
+  <dimension ref="A2:B20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
+      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -286,173 +307,122 @@
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>1</v>
-      </c>
+      <c r="A2" s="1"/>
+      <c r="B2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>4</v>
-      </c>
+      <c r="A3" s="1"/>
+      <c r="B3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1"/>
       <c r="B4" s="2"/>
-      <c r="C4" s="0" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1"/>
       <c r="B5" s="2"/>
-      <c r="C5" s="0" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="B6" s="1"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1"/>
+      <c r="B10" s="2"/>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="1"/>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="2" t="s">
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1"/>
-      <c r="B9" s="2"/>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3" t="s">
+      <c r="B13" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="1"/>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1"/>
-      <c r="B12" s="2"/>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1"/>
-      <c r="B13" s="2"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1"/>
       <c r="B14" s="2"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1"/>
-      <c r="B15" s="2"/>
+      <c r="A15" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="1"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1"/>
-      <c r="B16" s="2"/>
+      <c r="A16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1"/>
-      <c r="B17" s="2"/>
+      <c r="A17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1"/>
-      <c r="B18" s="2"/>
+      <c r="A18" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1"/>
-      <c r="B19" s="2"/>
+      <c r="A19" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1"/>
       <c r="B20" s="2"/>
-    </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1"/>
-      <c r="B21" s="2"/>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1"/>
-      <c r="B22" s="2"/>
-    </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1"/>
-      <c r="B23" s="2"/>
-    </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1"/>
-      <c r="B24" s="2"/>
-    </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1"/>
-      <c r="B25" s="2"/>
-    </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1"/>
-      <c r="B26" s="2"/>
-    </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="1"/>
-      <c r="B27" s="2"/>
-    </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="1"/>
-      <c r="B28" s="2"/>
-    </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="1"/>
-      <c r="B29" s="2"/>
-    </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="1"/>
-      <c r="B30" s="2"/>
-    </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="1"/>
-      <c r="B31" s="2"/>
-    </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="1"/>
-      <c r="B32" s="2"/>
-    </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="1"/>
-      <c r="B33" s="2"/>
-    </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="1"/>
-      <c r="B34" s="2"/>
-    </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="1"/>
-      <c r="B35" s="2"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
data-model: Add name to organisation
</commit_message>
<xml_diff>
--- a/indigo/spreadsheetform_guides/organisation.xlsx
+++ b/indigo/spreadsheetform_guides/organisation.xlsx
@@ -20,7 +20,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+  <si>
+    <t xml:space="preserve">Name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SPREADSHEETFORM:SINGLE:name/value</t>
+  </si>
   <si>
     <t xml:space="preserve">Org-Ids</t>
   </si>
@@ -44,9 +50,6 @@
   </si>
   <si>
     <t xml:space="preserve">Contact</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Name</t>
   </si>
   <si>
     <t xml:space="preserve">SPREADSHEETFORM:SINGLE:contact/name/value</t>
@@ -294,7 +297,7 @@
   <dimension ref="A2:B20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -307,8 +310,12 @@
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1"/>
-      <c r="B2" s="2"/>
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1"/>
@@ -324,32 +331,32 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B6" s="1"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -358,24 +365,24 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B11" s="1"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -384,40 +391,40 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B15" s="1"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
organisations: Add id to spreadsheet, like project has
</commit_message>
<xml_diff>
--- a/indigo/spreadsheetform_guides/organisation.xlsx
+++ b/indigo/spreadsheetform_guides/organisation.xlsx
@@ -20,7 +20,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
+  <si>
+    <t xml:space="preserve">SPREADSHEETFORM:SINGLE:id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Can not be changed)</t>
+  </si>
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -95,7 +101,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -116,6 +122,17 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="DejaVu Sans"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="DejaVu Sans"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -139,12 +156,24 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFEF413D"/>
+        <bgColor rgb="FF993366"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFCD3C1"/>
+        <bgColor rgb="FFE7E6E6"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -155,7 +184,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFE7E6E6"/>
-        <bgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFCD3C1"/>
       </patternFill>
     </fill>
   </fills>
@@ -200,7 +229,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -213,7 +242,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -267,13 +304,13 @@
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FFFCD3C1"/>
       <rgbColor rgb="FF2E75B6"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FFEF413D"/>
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF003366"/>
@@ -294,10 +331,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:B20"/>
+  <dimension ref="A2:C22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -310,126 +347,135 @@
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="1"/>
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="0" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1"/>
-      <c r="B3" s="2"/>
-    </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1"/>
-      <c r="B4" s="2"/>
+      <c r="A4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1"/>
-      <c r="B5" s="2"/>
+      <c r="A5" s="3"/>
+      <c r="B5" s="4"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="1"/>
+      <c r="A6" s="3"/>
+      <c r="B6" s="4"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="2" t="s">
+      <c r="A7" s="3"/>
+      <c r="B7" s="4"/>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
+      <c r="B8" s="3"/>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B9" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B10" s="4" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1"/>
-      <c r="B10" s="2"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="1"/>
+      <c r="B11" s="4" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>10</v>
-      </c>
+      <c r="A12" s="3"/>
+      <c r="B12" s="4"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="3"/>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1"/>
-      <c r="B14" s="2"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="1"/>
+      <c r="B15" s="4" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" s="2" t="s">
+      <c r="A16" s="3"/>
+      <c r="B16" s="4"/>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="5" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1" t="s">
+      <c r="B17" s="3"/>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B18" s="4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1" t="s">
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B19" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1" t="s">
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B20" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1"/>
-      <c r="B20" s="2"/>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="3"/>
+      <c r="B22" s="4"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>